<commit_message>
Add histogram to show weight distribution
</commit_message>
<xml_diff>
--- a/Quartiles, the IQR, and Percentiles/Workbook NBA players season 14-15.xlsx
+++ b/Quartiles, the IQR, and Percentiles/Workbook NBA players season 14-15.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Sites\WYWM_DataAnalysisExcel\Quartiles, the IQR, and Percentiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEE38B65-AC45-4BF4-BDF2-C4EA26C0A7BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13A63C95-2BBE-4881-8DFD-FF3409DCE085}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,12 +24,16 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'Classifying data'!$A$1:$B$423</definedName>
     <definedName name="_xlchart.v1.0" hidden="1">'NBA Players 14-15 season'!$F$1</definedName>
     <definedName name="_xlchart.v1.1" hidden="1">'NBA Players 14-15 season'!$F$2:$F$423</definedName>
+    <definedName name="_xlchart.v1.10" hidden="1">'NBA Players 14-15 season'!$F$1</definedName>
+    <definedName name="_xlchart.v1.11" hidden="1">'NBA Players 14-15 season'!$F$2:$F$423</definedName>
     <definedName name="_xlchart.v1.2" hidden="1">'NBA Players 14-15 season'!$F$1</definedName>
     <definedName name="_xlchart.v1.3" hidden="1">'NBA Players 14-15 season'!$F$2:$F$423</definedName>
     <definedName name="_xlchart.v1.4" hidden="1">'NBA Players 14-15 season'!$F$1</definedName>
     <definedName name="_xlchart.v1.5" hidden="1">'NBA Players 14-15 season'!$F$2:$F$423</definedName>
     <definedName name="_xlchart.v1.6" hidden="1">'NBA Players 14-15 season'!$F$1</definedName>
     <definedName name="_xlchart.v1.7" hidden="1">'NBA Players 14-15 season'!$F$2:$F$423</definedName>
+    <definedName name="_xlchart.v1.8" hidden="1">'NBA Players 14-15 season'!$F$1</definedName>
+    <definedName name="_xlchart.v1.9" hidden="1">'NBA Players 14-15 season'!$F$2:$F$423</definedName>
     <definedName name="ExternalData_1" localSheetId="0" hidden="1">Sheet2!$A$1:$G$423</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -2513,7 +2517,114 @@
 </cx:chartSpace>
 </file>
 
+<file path=xl/charts/chartEx2.xml><?xml version="1.0" encoding="utf-8"?>
+<cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
+  <cx:chartData>
+    <cx:data id="0">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.3</cx:f>
+      </cx:numDim>
+    </cx:data>
+  </cx:chartData>
+  <cx:chart>
+    <cx:title pos="t" align="ctr" overlay="0">
+      <cx:tx>
+        <cx:txData>
+          <cx:v>Frequency distribution weight</cx:v>
+        </cx:txData>
+      </cx:tx>
+      <cx:txPr>
+        <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:sysClr>
+              </a:solidFill>
+              <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+            </a:rPr>
+            <a:t>Frequency distribution weight</a:t>
+          </a:r>
+        </a:p>
+      </cx:txPr>
+    </cx:title>
+    <cx:plotArea>
+      <cx:plotAreaRegion>
+        <cx:series layoutId="clusteredColumn" uniqueId="{717D51E2-6318-483C-A22F-416D7514D6AC}">
+          <cx:tx>
+            <cx:txData>
+              <cx:f>_xlchart.v1.2</cx:f>
+              <cx:v>Weight</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:dataId val="0"/>
+          <cx:layoutPr>
+            <cx:binning intervalClosed="r"/>
+          </cx:layoutPr>
+        </cx:series>
+      </cx:plotAreaRegion>
+      <cx:axis id="0">
+        <cx:catScaling gapWidth="0"/>
+        <cx:tickLabels/>
+      </cx:axis>
+      <cx:axis id="1">
+        <cx:valScaling/>
+        <cx:majorGridlines/>
+        <cx:tickLabels/>
+      </cx:axis>
+    </cx:plotArea>
+  </cx:chart>
+</cx:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -3068,6 +3179,514 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="366">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat">
+        <a:solidFill>
+          <a:srgbClr val="D9D9D9"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -3079,9 +3698,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>392906</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:colOff>452438</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>148828</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
@@ -3118,7 +3737,85 @@
           <xdr:spPr>
             <a:xfrm>
               <a:off x="2952750" y="1446609"/>
-              <a:ext cx="2214562" cy="2743200"/>
+              <a:ext cx="2274094" cy="2244328"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-GB" sz="1100"/>
+                <a:t>This chart isn’t available in your version of Excel.
+Editing this shape or saving this workbook into a different file format will permanently break the chart.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>303609</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>321469</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="3" name="Chart 2">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F1C1BAE2-3CCD-4790-8DC3-20B10EA0EBCB}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2014/chartex">
+              <cx:chart xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="5381625" y="1446609"/>
+              <a:ext cx="4572000" cy="2743200"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -13598,8 +14295,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7316473-FC0A-4C63-BA86-386CFCDD993B}">
   <dimension ref="B2:M17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15:XFD15"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Show spread of player scores
</commit_message>
<xml_diff>
--- a/Quartiles, the IQR, and Percentiles/Workbook NBA players season 14-15.xlsx
+++ b/Quartiles, the IQR, and Percentiles/Workbook NBA players season 14-15.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Sites\WYWM_DataAnalysisExcel\Quartiles, the IQR, and Percentiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13A63C95-2BBE-4881-8DFD-FF3409DCE085}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{845E2FBC-7BB6-4F36-B8D2-391B89E96821}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="3" state="hidden" r:id="rId1"/>
@@ -26,14 +26,26 @@
     <definedName name="_xlchart.v1.1" hidden="1">'NBA Players 14-15 season'!$F$2:$F$423</definedName>
     <definedName name="_xlchart.v1.10" hidden="1">'NBA Players 14-15 season'!$F$1</definedName>
     <definedName name="_xlchart.v1.11" hidden="1">'NBA Players 14-15 season'!$F$2:$F$423</definedName>
+    <definedName name="_xlchart.v1.12" hidden="1">'NBA Players 14-15 season'!$C$1</definedName>
+    <definedName name="_xlchart.v1.13" hidden="1">'NBA Players 14-15 season'!$C$2:$C$423</definedName>
+    <definedName name="_xlchart.v1.14" hidden="1">'NBA Players 14-15 season'!$F$1</definedName>
+    <definedName name="_xlchart.v1.15" hidden="1">'NBA Players 14-15 season'!$F$2:$F$423</definedName>
+    <definedName name="_xlchart.v1.16" hidden="1">'NBA Players 14-15 season'!$F$1</definedName>
+    <definedName name="_xlchart.v1.17" hidden="1">'NBA Players 14-15 season'!$F$2:$F$423</definedName>
+    <definedName name="_xlchart.v1.18" hidden="1">'NBA Players 14-15 season'!$C$1</definedName>
+    <definedName name="_xlchart.v1.19" hidden="1">'NBA Players 14-15 season'!$C$2:$C$423</definedName>
     <definedName name="_xlchart.v1.2" hidden="1">'NBA Players 14-15 season'!$F$1</definedName>
+    <definedName name="_xlchart.v1.20" hidden="1">'NBA Players 14-15 season'!$F$1</definedName>
+    <definedName name="_xlchart.v1.21" hidden="1">'NBA Players 14-15 season'!$F$2:$F$423</definedName>
+    <definedName name="_xlchart.v1.22" hidden="1">'NBA Players 14-15 season'!$C$1</definedName>
+    <definedName name="_xlchart.v1.23" hidden="1">'NBA Players 14-15 season'!$C$2:$C$423</definedName>
     <definedName name="_xlchart.v1.3" hidden="1">'NBA Players 14-15 season'!$F$2:$F$423</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">'NBA Players 14-15 season'!$F$1</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">'NBA Players 14-15 season'!$F$2:$F$423</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">'NBA Players 14-15 season'!$F$1</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">'NBA Players 14-15 season'!$F$2:$F$423</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">'NBA Players 14-15 season'!$F$1</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">'NBA Players 14-15 season'!$F$2:$F$423</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">'NBA Players 14-15 season'!$C$1</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">'NBA Players 14-15 season'!$C$2:$C$423</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">'NBA Players 14-15 season'!$C$1</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">'NBA Players 14-15 season'!$C$2:$C$423</definedName>
+    <definedName name="_xlchart.v1.8" hidden="1">'NBA Players 14-15 season'!$C$1</definedName>
+    <definedName name="_xlchart.v1.9" hidden="1">'NBA Players 14-15 season'!$C$2:$C$423</definedName>
     <definedName name="ExternalData_1" localSheetId="0" hidden="1">Sheet2!$A$1:$G$423</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -71,7 +83,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1358" uniqueCount="487">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1363" uniqueCount="492">
   <si>
     <t>Name</t>
   </si>
@@ -1534,6 +1546,21 @@
   </si>
   <si>
     <t>Lower Out Q1-Out</t>
+  </si>
+  <si>
+    <t>Outlier</t>
+  </si>
+  <si>
+    <t>Upper Outlier</t>
+  </si>
+  <si>
+    <t>Lower Outlier</t>
+  </si>
+  <si>
+    <t>Mean</t>
+  </si>
+  <si>
+    <t>Median</t>
   </si>
 </sst>
 </file>
@@ -2584,6 +2611,141 @@
 </cx:chartSpace>
 </file>
 
+<file path=xl/charts/chartEx3.xml><?xml version="1.0" encoding="utf-8"?>
+<cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
+  <cx:chartData>
+    <cx:data id="0">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.7</cx:f>
+      </cx:numDim>
+    </cx:data>
+  </cx:chartData>
+  <cx:chart>
+    <cx:title pos="t" align="ctr" overlay="0">
+      <cx:tx>
+        <cx:txData>
+          <cx:v>Points scored</cx:v>
+        </cx:txData>
+      </cx:tx>
+      <cx:txPr>
+        <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:sysClr>
+              </a:solidFill>
+              <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+            </a:rPr>
+            <a:t>Points scored</a:t>
+          </a:r>
+        </a:p>
+      </cx:txPr>
+    </cx:title>
+    <cx:plotArea>
+      <cx:plotAreaRegion>
+        <cx:series layoutId="clusteredColumn" uniqueId="{C929FA82-D055-474B-8B70-ED836EC09034}">
+          <cx:tx>
+            <cx:txData>
+              <cx:f>_xlchart.v1.6</cx:f>
+              <cx:v>PTS</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:dataId val="0"/>
+          <cx:layoutPr>
+            <cx:binning intervalClosed="r"/>
+          </cx:layoutPr>
+        </cx:series>
+      </cx:plotAreaRegion>
+      <cx:axis id="0">
+        <cx:catScaling gapWidth="0"/>
+        <cx:tickLabels/>
+      </cx:axis>
+      <cx:axis id="1">
+        <cx:valScaling/>
+        <cx:majorGridlines/>
+        <cx:tickLabels/>
+      </cx:axis>
+    </cx:plotArea>
+  </cx:chart>
+</cx:chartSpace>
+</file>
+
+<file path=xl/charts/chartEx4.xml><?xml version="1.0" encoding="utf-8"?>
+<cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
+  <cx:chartData>
+    <cx:data id="0">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.5</cx:f>
+      </cx:numDim>
+    </cx:data>
+  </cx:chartData>
+  <cx:chart>
+    <cx:title pos="t" align="ctr" overlay="0">
+      <cx:tx>
+        <cx:txData>
+          <cx:v>Points scored</cx:v>
+        </cx:txData>
+      </cx:tx>
+      <cx:txPr>
+        <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:sysClr>
+              </a:solidFill>
+              <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+            </a:rPr>
+            <a:t>Points scored</a:t>
+          </a:r>
+        </a:p>
+      </cx:txPr>
+    </cx:title>
+    <cx:plotArea>
+      <cx:plotAreaRegion>
+        <cx:series layoutId="boxWhisker" uniqueId="{52D98E66-5F03-4ADE-BEA4-CAB9B5D505F5}">
+          <cx:tx>
+            <cx:txData>
+              <cx:f>_xlchart.v1.4</cx:f>
+              <cx:v>PTS</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:dataId val="0"/>
+          <cx:layoutPr>
+            <cx:visibility meanLine="0" meanMarker="1" nonoutliers="0" outliers="1"/>
+            <cx:statistics quartileMethod="exclusive"/>
+          </cx:layoutPr>
+        </cx:series>
+      </cx:plotAreaRegion>
+      <cx:axis id="0">
+        <cx:catScaling gapWidth="1"/>
+        <cx:tickLabels/>
+      </cx:axis>
+      <cx:axis id="1">
+        <cx:valScaling/>
+        <cx:majorGridlines/>
+        <cx:tickLabels/>
+      </cx:axis>
+    </cx:plotArea>
+  </cx:chart>
+</cx:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -2625,6 +2787,86 @@
 </file>
 
 <file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -3687,6 +3929,1029 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="366">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat">
+        <a:solidFill>
+          <a:srgbClr val="D9D9D9"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="406">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat">
+        <a:solidFill>
+          <a:srgbClr val="D9D9D9"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -3849,6 +5114,167 @@
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>321469</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>189309</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="3" name="Chart 2">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E01D1A5C-8036-40E4-8079-A7065F34BDCD}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2014/chartex">
+              <cx:chart xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="5893594" y="1375172"/>
+              <a:ext cx="4572000" cy="2743200"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-GB" sz="1100"/>
+                <a:t>This chart isn’t available in your version of Excel.
+Editing this shape or saving this workbook into a different file format will permanently break the chart.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>577453</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>136921</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="4" name="Chart 3">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4B7A93A4-9630-4F79-99A6-88A3DF290D22}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2014/chartex">
+              <cx:chart xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="2250281" y="1375172"/>
+              <a:ext cx="3006328" cy="2500312"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-GB" sz="1100"/>
+                <a:t>This chart isn’t available in your version of Excel.
+Editing this shape or saving this workbook into a different file format will permanently break the chart.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -14295,7 +15721,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7316473-FC0A-4C63-BA86-386CFCDD993B}">
   <dimension ref="B2:M17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
@@ -14471,10 +15897,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A25B489-0AFC-48AF-9DC6-D8CC84A91864}">
-  <dimension ref="B1:M18"/>
+  <dimension ref="B1:M22"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14520,7 +15946,10 @@
       <c r="B8" s="14" t="s">
         <v>445</v>
       </c>
-      <c r="C8" s="12"/>
+      <c r="C8" s="12">
+        <f>QUARTILE('NBA Players 14-15 season'!C:C,1)</f>
+        <v>154.25</v>
+      </c>
     </row>
     <row r="9" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B9" s="14"/>
@@ -14530,7 +15959,10 @@
       <c r="B10" s="14" t="s">
         <v>446</v>
       </c>
-      <c r="C10" s="12"/>
+      <c r="C10" s="12">
+        <f>QUARTILE('NBA Players 14-15 season'!C:C,2)</f>
+        <v>432</v>
+      </c>
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B11" s="14"/>
@@ -14540,7 +15972,10 @@
       <c r="B12" s="14" t="s">
         <v>447</v>
       </c>
-      <c r="C12" s="12"/>
+      <c r="C12" s="12">
+        <f>QUARTILE('NBA Players 14-15 season'!C:C,3)</f>
+        <v>788.75</v>
+      </c>
     </row>
     <row r="13" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B13" s="14"/>
@@ -14550,14 +15985,61 @@
       <c r="B14" s="14" t="s">
         <v>450</v>
       </c>
-      <c r="C14" s="15"/>
+      <c r="C14" s="15">
+        <f>C12-C8</f>
+        <v>634.5</v>
+      </c>
     </row>
     <row r="15" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B15" s="14"/>
       <c r="C15" s="16"/>
     </row>
-    <row r="17" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="18" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>487</v>
+      </c>
+      <c r="C16">
+        <f>C14*1.5</f>
+        <v>951.75</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>488</v>
+      </c>
+      <c r="C17">
+        <f>C12+C16</f>
+        <v>1740.5</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>489</v>
+      </c>
+      <c r="C19">
+        <f>C8-C14</f>
+        <v>-480.25</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>490</v>
+      </c>
+      <c r="C21">
+        <f>AVERAGE('NBA Players 14-15 season'!C:C)</f>
+        <v>515.89099526066354</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>491</v>
+      </c>
+      <c r="C22">
+        <f>MEDIAN('NBA Players 14-15 season'!C:C)</f>
+        <v>432</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="9">
     <mergeCell ref="B12:B13"/>
@@ -14572,6 +16054,7 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -18298,7 +19781,7 @@
   <dimension ref="A1:G423"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F1048576"/>
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>